<commit_message>
Added Earlier years to training AFL Best is 71.36% at H= {L=1, N=5}
</commit_message>
<xml_diff>
--- a/tipper/bin/Debug/Success_vs_time.xlsx
+++ b/tipper/bin/Debug/Success_vs_time.xlsx
@@ -7,17 +7,16 @@
     <workbookView xWindow="480" yWindow="45" windowWidth="13395" windowHeight="8265"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Training-Testing Overlap found" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Layers</t>
   </si>
@@ -369,10 +368,1628 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>66.83</v>
+      </c>
+      <c r="E2">
+        <v>17.641999999999999</v>
+      </c>
+      <c r="F2">
+        <f>IF(D2&gt;=MAX(D:D), 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>65.33</v>
+      </c>
+      <c r="E3">
+        <v>71.031999999999996</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">IF(D3&gt;=MAX(D:D), 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <f t="shared" ref="A4:A67" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>64.319999999999993</v>
+      </c>
+      <c r="E4">
+        <v>175.49799999999999</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>64.319999999999993</v>
+      </c>
+      <c r="E5">
+        <v>386.44400000000002</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>64.819999999999993</v>
+      </c>
+      <c r="E6">
+        <v>548.40899999999999</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>66.33</v>
+      </c>
+      <c r="E7">
+        <v>28.125</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>63.82</v>
+      </c>
+      <c r="E8">
+        <v>54.174999999999997</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>62.31</v>
+      </c>
+      <c r="E9">
+        <v>114.34</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>67.84</v>
+      </c>
+      <c r="E10">
+        <v>50.136000000000003</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>68.34</v>
+      </c>
+      <c r="E11">
+        <v>247.76599999999999</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>68.84</v>
+      </c>
+      <c r="E12">
+        <v>250.08099999999999</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>68.34</v>
+      </c>
+      <c r="E13">
+        <v>765.11400000000003</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>58.79</v>
+      </c>
+      <c r="E14">
+        <v>38.287999999999997</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>65.33</v>
+      </c>
+      <c r="E15">
+        <v>128.279</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>67.34</v>
+      </c>
+      <c r="E16">
+        <v>282.17099999999999</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>67.34</v>
+      </c>
+      <c r="E17">
+        <v>543.46400000000006</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>68.34</v>
+      </c>
+      <c r="E18">
+        <v>126.75</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>67.84</v>
+      </c>
+      <c r="E19">
+        <v>842.1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>68.34</v>
+      </c>
+      <c r="E20">
+        <v>1301.354</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>68.34</v>
+      </c>
+      <c r="E21">
+        <v>1781.152</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>57.29</v>
+      </c>
+      <c r="E22">
+        <v>44.271000000000001</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>69.349999999999994</v>
+      </c>
+      <c r="E23">
+        <v>157.81</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>67.34</v>
+      </c>
+      <c r="E24">
+        <v>388.44099999999997</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>70.349999999999994</v>
+      </c>
+      <c r="E25">
+        <v>857.53899999999999</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>67.84</v>
+      </c>
+      <c r="E26">
+        <v>18.3</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>66.83</v>
+      </c>
+      <c r="E27">
+        <v>102.17</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>66.83</v>
+      </c>
+      <c r="E28">
+        <v>132.04599999999999</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>67.34</v>
+      </c>
+      <c r="E29">
+        <v>232.381</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>67.34</v>
+      </c>
+      <c r="E30">
+        <v>292.34500000000003</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>59.8</v>
+      </c>
+      <c r="E31">
+        <v>92.808999999999997</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>66.33</v>
+      </c>
+      <c r="E32">
+        <v>71.475999999999999</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>65.83</v>
+      </c>
+      <c r="E33">
+        <v>153.876</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>66.33</v>
+      </c>
+      <c r="E34">
+        <v>384.197</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>65.83</v>
+      </c>
+      <c r="E35">
+        <v>630.86599999999999</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>68.84</v>
+      </c>
+      <c r="E36">
+        <v>18.3</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>66.83</v>
+      </c>
+      <c r="E37">
+        <v>106.96</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>67.34</v>
+      </c>
+      <c r="E38">
+        <v>131.60599999999999</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>67.84</v>
+      </c>
+      <c r="E39">
+        <v>160.268</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>67.84</v>
+      </c>
+      <c r="E40">
+        <v>184.386</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>68.34</v>
+      </c>
+      <c r="E41">
+        <v>258.88499999999999</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <v>68.84</v>
+      </c>
+      <c r="E42">
+        <v>410.952</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>66.33</v>
+      </c>
+      <c r="E43">
+        <v>525.39099999999996</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>66.33</v>
+      </c>
+      <c r="E44">
+        <v>6.4880000000000004</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>65.83</v>
+      </c>
+      <c r="E45">
+        <v>26.143000000000001</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>67.34</v>
+      </c>
+      <c r="E46">
+        <v>69.628</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>67.84</v>
+      </c>
+      <c r="E47">
+        <v>152.81200000000001</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>68.34</v>
+      </c>
+      <c r="E48">
+        <v>284.94900000000001</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>6</v>
+      </c>
+      <c r="D49">
+        <v>67.84</v>
+      </c>
+      <c r="E49">
+        <v>466.06799999999998</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>67.84</v>
+      </c>
+      <c r="E50">
+        <v>720.41600000000005</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>8</v>
+      </c>
+      <c r="D51">
+        <v>67.34</v>
+      </c>
+      <c r="E51">
+        <v>1024.8579999999999</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>55.28</v>
+      </c>
+      <c r="E52">
+        <v>17.471</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>55.28</v>
+      </c>
+      <c r="E53">
+        <v>190.119</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>55.28</v>
+      </c>
+      <c r="E54">
+        <v>276.77100000000002</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <v>56.28</v>
+      </c>
+      <c r="E55">
+        <v>623.10500000000002</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>66.33</v>
+      </c>
+      <c r="E56">
+        <v>56.890999999999998</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>67.84</v>
+      </c>
+      <c r="E57">
+        <v>510.358</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <v>68.84</v>
+      </c>
+      <c r="E58">
+        <v>1345.4380000000001</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59">
+        <v>68.34</v>
+      </c>
+      <c r="E59">
+        <v>1791.413</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
+      </c>
+      <c r="D60">
+        <v>68.34</v>
+      </c>
+      <c r="E60">
+        <v>2267.9929999999999</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>65.33</v>
+      </c>
+      <c r="E61">
+        <v>43.264000000000003</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>65.33</v>
+      </c>
+      <c r="E62">
+        <v>151.44800000000001</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <v>64.819999999999993</v>
+      </c>
+      <c r="E63">
+        <v>345.75799999999998</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>65.83</v>
+      </c>
+      <c r="E64">
+        <v>704.74699999999996</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>66.83</v>
+      </c>
+      <c r="E65">
+        <v>1267.8209999999999</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>69.849999999999994</v>
+      </c>
+      <c r="E66">
+        <v>153.52500000000001</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>70.849999999999994</v>
+      </c>
+      <c r="E67">
+        <v>310.66500000000002</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F73" si="2">IF(D67&gt;=MAX(D:D), 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68">
+        <f t="shared" ref="A68:A73" si="3">A67+1</f>
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68">
+        <v>69.849999999999994</v>
+      </c>
+      <c r="E68">
+        <v>1668.463</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>67.84</v>
+      </c>
+      <c r="E69">
+        <v>2278.049</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+      <c r="D70">
+        <v>71.36</v>
+      </c>
+      <c r="E70">
+        <v>2490.4780000000001</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>65.33</v>
+      </c>
+      <c r="E71">
+        <v>49.527000000000001</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <v>66.33</v>
+      </c>
+      <c r="E72">
+        <v>179.93600000000001</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73">
+        <v>66.83</v>
+      </c>
+      <c r="E73">
+        <v>432.86799999999999</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I114" sqref="I114"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3504,18 +5121,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>